<commit_message>
Push up set value (#7)
* .

* Update RenderExcel.cs
</commit_message>
<xml_diff>
--- a/src/ExcelsiorAspose.Tests/NullableTests.NullDisplay.verified.xlsx
+++ b/src/ExcelsiorAspose.Tests/NullableTests.NullDisplay.verified.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Number</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>True</t>
   </si>
 </sst>
 </file>
@@ -561,8 +558,8 @@
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
+      <c r="E3" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add date only support (#9)
</commit_message>
<xml_diff>
--- a/src/ExcelsiorAspose.Tests/NullableTests.NullDisplay.verified.xlsx
+++ b/src/ExcelsiorAspose.Tests/NullableTests.NullDisplay.verified.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$3</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Number</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Date Time</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>Enum</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
   </si>
   <si>
     <t>[No DateTime]</t>
+  </si>
+  <si>
+    <t>[No Date]</t>
   </si>
   <si>
     <t>[No Enum]</t>
@@ -62,8 +68,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="177" formatCode="yyyy-MM-dd"/>
+    <numFmt numFmtId="178" formatCode="yyyy-MM-dd HH:mm:ss"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -101,9 +108,12 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -494,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -506,12 +516,13 @@
   <cols>
     <col min="1" max="1" width="12.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="10.7142857142857" customWidth="1"/>
-    <col min="3" max="3" width="13.7142857142857" customWidth="1"/>
-    <col min="4" max="4" width="10.7142857142857" customWidth="1"/>
-    <col min="5" max="5" width="9.71428571428571" customWidth="1"/>
+    <col min="3" max="3" width="18.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="11.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="10.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="9.71428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14" customHeight="1">
+    <row r="1" spans="1:6" ht="14" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,43 +538,52 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="14" customHeight="1">
+    <row r="2" spans="1:6" ht="14" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" customHeight="1">
+    <row r="3" spans="1:6" ht="14" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2">
+        <v>43831.427141203705</v>
+      </c>
+      <c r="D3" s="3">
         <v>43831</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="b">
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E3"/>
+  <autoFilter ref="A1:F3"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>